<commit_message>
New calculation matching, Restructured result function and sheet
</commit_message>
<xml_diff>
--- a/SFTestData.xlsx
+++ b/SFTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enayem\Documents\DTC_katalon - V.4.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B539B8-1171-4D48-BAD4-F3C33735D56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27EC4C4-2A97-4E58-8F4F-8894AEE6AFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="449" activeTab="3" xr2:uid="{16B02AFA-F9A7-40B3-B18D-728772148A96}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="449" firstSheet="3" activeTab="4" xr2:uid="{16B02AFA-F9A7-40B3-B18D-728772148A96}"/>
   </bookViews>
   <sheets>
     <sheet name="GM_TD" sheetId="13" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="388">
   <si>
     <t>TestCase</t>
   </si>
@@ -672,9 +672,6 @@
     <t>0065500000M8PVYAA3</t>
   </si>
   <si>
-    <t>ganeshsase2020+3163@gmail.com</t>
-  </si>
-  <si>
     <t>00000SC2</t>
   </si>
   <si>
@@ -978,12 +975,6 @@
     <t>mai</t>
   </si>
   <si>
-    <t>5UX53DP03N9M29144</t>
-  </si>
-  <si>
-    <t>xyzab</t>
-  </si>
-  <si>
     <t>Portal</t>
   </si>
   <si>
@@ -1113,10 +1104,109 @@
     <t>emrannayemd2c+001@gmail.com</t>
   </si>
   <si>
-    <t>1GKS2DKL0NR255756</t>
-  </si>
-  <si>
-    <t>006Ov000004MTEPIA4</t>
+    <t>5 year\(s\) or 60,000 kilometers</t>
+  </si>
+  <si>
+    <t>1GKS2DKL0NR255875</t>
+  </si>
+  <si>
+    <t>regression 6.2.1</t>
+  </si>
+  <si>
+    <t>006Ov000004MTEQIA4</t>
+  </si>
+  <si>
+    <t>ganeshsase2020+4515@gmail.com</t>
+  </si>
+  <si>
+    <t>006Ov000004MTEOIA4</t>
+  </si>
+  <si>
+    <t>7 year\(s\) or 100,000 kilometers</t>
+  </si>
+  <si>
+    <t>ganeshsase2020+4516@gmail.com</t>
+  </si>
+  <si>
+    <t>006Ov000004MTENIA4</t>
+  </si>
+  <si>
+    <t>2 year\(s\) or 48,000 kilometers</t>
+  </si>
+  <si>
+    <t>ganeshsase2020+4517@gmail.com</t>
+  </si>
+  <si>
+    <t>006Ov000004MTEMIA4</t>
+  </si>
+  <si>
+    <t>4 year\(s\) or 96,000 kilometers</t>
+  </si>
+  <si>
+    <t>ganeshsase2020+4518@gmail.com</t>
+  </si>
+  <si>
+    <t>WA1EVBF10ND005521</t>
+  </si>
+  <si>
+    <t>ganeshsase2020+4511@gmail.com</t>
+  </si>
+  <si>
+    <t>Same as primary Address</t>
+  </si>
+  <si>
+    <t>0065500000MnVeGAAV</t>
+  </si>
+  <si>
+    <t>Powertain</t>
+  </si>
+  <si>
+    <t>1 YEARS, 12,000 MILES</t>
+  </si>
+  <si>
+    <t>ganeshsase2020+4512@gmail.com</t>
+  </si>
+  <si>
+    <t>4 YEARS, 48,000 MILES</t>
+  </si>
+  <si>
+    <t>ganeshsase2020+4513@gmail.com</t>
+  </si>
+  <si>
+    <t>00000SC9</t>
+  </si>
+  <si>
+    <t>xyz12</t>
+  </si>
+  <si>
+    <t>5FNYF5H20NB014719</t>
+  </si>
+  <si>
+    <t>ganeshsase2020+4521@gmail.com</t>
+  </si>
+  <si>
+    <t>9876543210'</t>
+  </si>
+  <si>
+    <t>0000SC12</t>
+  </si>
+  <si>
+    <t>1abcd</t>
+  </si>
+  <si>
+    <t>5NPLM4AG7NH086020</t>
+  </si>
+  <si>
+    <t>ganeshsase2020+4522@gmail.com</t>
+  </si>
+  <si>
+    <t>Emran Test</t>
+  </si>
+  <si>
+    <t>5FNYF5H20NB014245</t>
+  </si>
+  <si>
+    <t>0065500000MieFTAAZ</t>
   </si>
 </sst>
 </file>
@@ -1729,7 +1819,7 @@
     <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1767,6 +1857,25 @@
     </xf>
     <xf numFmtId="0" fontId="28" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -2128,10 +2237,13 @@
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" t="s">
@@ -2219,7 +2331,7 @@
         <v>131</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="F2" s="7">
         <v>10000</v>
@@ -2228,7 +2340,7 @@
         <v>27</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I2">
         <v>100</v>
@@ -2240,22 +2352,22 @@
         <v>173</v>
       </c>
       <c r="M2" t="s">
-        <v>259</v>
+        <v>146</v>
       </c>
       <c r="N2" t="s">
+        <v>211</v>
+      </c>
+      <c r="O2" t="s">
         <v>212</v>
       </c>
-      <c r="O2" t="s">
-        <v>213</v>
-      </c>
       <c r="P2" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="Q2" s="3">
         <v>9999999999</v>
       </c>
       <c r="R2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="S2" t="s">
         <v>170</v>
@@ -2273,7 +2385,7 @@
         <v>999</v>
       </c>
       <c r="X2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -2288,10 +2400,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA2C7D7-980A-4C62-88D3-012EB065DEFC}">
-  <dimension ref="A1:AT140"/>
+  <dimension ref="A1:AT153"/>
   <sheetViews>
-    <sheetView topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="A140" sqref="A140:AT140"/>
+    <sheetView topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="A152" sqref="A152:AC153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3398,7 +3510,7 @@
     </row>
     <row r="47" spans="2:24">
       <c r="N47" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="O47" t="s">
         <v>208</v>
@@ -3415,7 +3527,7 @@
         <v>190</v>
       </c>
       <c r="F50" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G50" s="7">
         <v>48001</v>
@@ -3436,10 +3548,10 @@
         <v>187</v>
       </c>
       <c r="O50" t="s">
+        <v>211</v>
+      </c>
+      <c r="P50" t="s">
         <v>212</v>
-      </c>
-      <c r="P50" t="s">
-        <v>213</v>
       </c>
       <c r="Q50" s="1" t="s">
         <v>188</v>
@@ -3481,7 +3593,7 @@
         <v>131</v>
       </c>
       <c r="F51" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G51" s="7">
         <v>10000</v>
@@ -3505,10 +3617,10 @@
         <v>52</v>
       </c>
       <c r="O51" t="s">
+        <v>211</v>
+      </c>
+      <c r="P51" t="s">
         <v>212</v>
-      </c>
-      <c r="P51" t="s">
-        <v>213</v>
       </c>
       <c r="Q51" s="1" t="s">
         <v>188</v>
@@ -3526,7 +3638,7 @@
         <v>19</v>
       </c>
       <c r="V51" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="W51">
         <v>2030</v>
@@ -3549,7 +3661,7 @@
         <v>131</v>
       </c>
       <c r="F52" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G52" s="7">
         <v>5000</v>
@@ -3573,10 +3685,10 @@
         <v>52</v>
       </c>
       <c r="O52" t="s">
+        <v>211</v>
+      </c>
+      <c r="P52" t="s">
         <v>212</v>
-      </c>
-      <c r="P52" t="s">
-        <v>213</v>
       </c>
       <c r="Q52" s="1" t="s">
         <v>188</v>
@@ -3594,7 +3706,7 @@
         <v>19</v>
       </c>
       <c r="V52" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="W52">
         <v>2030</v>
@@ -3608,7 +3720,7 @@
     </row>
     <row r="55" spans="2:29" ht="28.8">
       <c r="B55" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="56" spans="2:29" ht="16.8">
@@ -3616,10 +3728,10 @@
         <v>148</v>
       </c>
       <c r="D56" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E56" s="13" t="s">
         <v>220</v>
-      </c>
-      <c r="E56" s="13" t="s">
-        <v>221</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>130</v>
@@ -3632,7 +3744,7 @@
         <v>27</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="L56" s="3"/>
       <c r="M56" s="3"/>
@@ -3649,7 +3761,7 @@
         <v>184</v>
       </c>
       <c r="R56" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S56" s="8">
         <v>4044063049</v>
@@ -3673,7 +3785,7 @@
         <v>121</v>
       </c>
       <c r="Z56" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="57" spans="2:29" ht="16.8">
@@ -3681,13 +3793,13 @@
         <v>148</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E57" t="s">
+        <v>224</v>
+      </c>
+      <c r="F57" t="s">
         <v>225</v>
-      </c>
-      <c r="F57" t="s">
-        <v>226</v>
       </c>
       <c r="H57">
         <v>10000</v>
@@ -3696,7 +3808,7 @@
         <v>25</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="O57" t="s">
         <v>143</v>
@@ -3708,13 +3820,13 @@
         <v>184</v>
       </c>
       <c r="R57" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="S57" s="8">
         <v>4044063049</v>
       </c>
       <c r="T57" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="U57" s="3" t="s">
         <v>185</v>
@@ -3743,7 +3855,7 @@
         <v>181</v>
       </c>
       <c r="E60" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>130</v>
@@ -3753,10 +3865,10 @@
         <v>2000</v>
       </c>
       <c r="I60" t="s">
+        <v>230</v>
+      </c>
+      <c r="J60" s="3" t="s">
         <v>231</v>
-      </c>
-      <c r="J60" s="3" t="s">
-        <v>232</v>
       </c>
       <c r="O60" s="3" t="s">
         <v>128</v>
@@ -3768,7 +3880,7 @@
         <v>184</v>
       </c>
       <c r="R60" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="S60" s="8">
         <v>4044063049</v>
@@ -3792,7 +3904,7 @@
         <v>121</v>
       </c>
       <c r="Z60" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="61" spans="2:29" ht="16.8">
@@ -3803,19 +3915,19 @@
         <v>181</v>
       </c>
       <c r="E61" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F61" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H61">
         <v>10000</v>
       </c>
       <c r="I61" t="s">
+        <v>234</v>
+      </c>
+      <c r="J61" s="3" t="s">
         <v>235</v>
-      </c>
-      <c r="J61" s="3" t="s">
-        <v>236</v>
       </c>
       <c r="O61" t="s">
         <v>143</v>
@@ -3827,13 +3939,13 @@
         <v>184</v>
       </c>
       <c r="R61" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="S61" s="8">
         <v>4044063049</v>
       </c>
       <c r="T61" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="U61" s="3" t="s">
         <v>185</v>
@@ -3862,13 +3974,13 @@
         <v>177</v>
       </c>
       <c r="D63" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="E63" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="E63" s="7" t="s">
-        <v>211</v>
-      </c>
       <c r="G63" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H63">
         <v>24001</v>
@@ -3898,7 +4010,7 @@
         <v>184</v>
       </c>
       <c r="S63" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="T63" s="8">
         <v>1111111111</v>
@@ -3922,7 +4034,7 @@
         <v>121</v>
       </c>
       <c r="AA63" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AC63" s="14"/>
     </row>
@@ -3931,13 +4043,13 @@
         <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E65" t="s">
         <v>208</v>
       </c>
       <c r="F65" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H65">
         <v>36001</v>
@@ -3955,7 +4067,7 @@
         <v>29</v>
       </c>
       <c r="O65" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P65" s="3" t="s">
         <v>183</v>
@@ -3964,13 +4076,13 @@
         <v>184</v>
       </c>
       <c r="R65" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="S65" s="8">
         <v>1111111112</v>
       </c>
       <c r="T65" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="U65" s="3" t="s">
         <v>185</v>
@@ -3988,7 +4100,7 @@
         <v>121</v>
       </c>
       <c r="Z65" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="67" spans="1:28" ht="18.600000000000001">
@@ -4002,7 +4114,7 @@
         <v>131</v>
       </c>
       <c r="G67" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H67">
         <v>24001</v>
@@ -4029,7 +4141,7 @@
         <v>184</v>
       </c>
       <c r="R67" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="S67" s="8">
         <v>1111111112</v>
@@ -4069,7 +4181,7 @@
         <v>131</v>
       </c>
       <c r="F70" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G70" s="7">
         <v>10000</v>
@@ -4078,7 +4190,7 @@
         <v>27</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J70">
         <v>0</v>
@@ -4099,7 +4211,7 @@
         <v>184</v>
       </c>
       <c r="Q70" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="R70" s="3">
         <v>9999999999</v>
@@ -4134,7 +4246,7 @@
         <v>109</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E72" t="s">
         <v>190</v>
@@ -4167,7 +4279,7 @@
         <v>184</v>
       </c>
       <c r="Q72" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="R72" s="3">
         <v>9999999999</v>
@@ -4191,7 +4303,7 @@
         <v>999</v>
       </c>
       <c r="Y72" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="74" spans="1:28">
@@ -4206,7 +4318,7 @@
         <v>131</v>
       </c>
       <c r="F74" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G74" s="7">
         <v>10000</v>
@@ -4215,7 +4327,7 @@
         <v>68</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J74">
         <v>250</v>
@@ -4224,7 +4336,7 @@
         <v>180</v>
       </c>
       <c r="N74" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="O74" t="s">
         <v>183</v>
@@ -4233,7 +4345,7 @@
         <v>184</v>
       </c>
       <c r="Q74" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="R74" s="3">
         <v>9999999999</v>
@@ -4271,7 +4383,7 @@
         <v>131</v>
       </c>
       <c r="F76" s="17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G76" s="7">
         <v>1000</v>
@@ -4280,7 +4392,7 @@
         <v>27</v>
       </c>
       <c r="I76" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J76">
         <v>0</v>
@@ -4298,7 +4410,7 @@
         <v>184</v>
       </c>
       <c r="Q76" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="R76" s="3">
         <v>9999999999</v>
@@ -4337,7 +4449,7 @@
         <v>131</v>
       </c>
       <c r="E80" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F80" s="7">
         <v>10000</v>
@@ -4346,19 +4458,19 @@
         <v>27</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I80">
         <v>100</v>
       </c>
       <c r="M80" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="N80" t="s">
+        <v>211</v>
+      </c>
+      <c r="O80" t="s">
         <v>212</v>
-      </c>
-      <c r="O80" t="s">
-        <v>213</v>
       </c>
       <c r="P80" s="1" t="s">
         <v>188</v>
@@ -4367,7 +4479,7 @@
         <v>9999999999</v>
       </c>
       <c r="R80" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="S80" t="s">
         <v>170</v>
@@ -4385,7 +4497,7 @@
         <v>999</v>
       </c>
       <c r="X80" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="81" spans="1:24">
@@ -4399,7 +4511,7 @@
         <v>161</v>
       </c>
       <c r="E81" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F81">
         <v>2000</v>
@@ -4408,7 +4520,7 @@
         <v>27</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I81">
         <v>0</v>
@@ -4417,10 +4529,10 @@
         <v>187</v>
       </c>
       <c r="N81" t="s">
+        <v>211</v>
+      </c>
+      <c r="O81" t="s">
         <v>212</v>
-      </c>
-      <c r="O81" t="s">
-        <v>213</v>
       </c>
       <c r="P81" s="1" t="s">
         <v>188</v>
@@ -4429,7 +4541,7 @@
         <v>9999999999</v>
       </c>
       <c r="R81" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="S81" t="s">
         <v>170</v>
@@ -4438,7 +4550,7 @@
         <v>19</v>
       </c>
       <c r="U81" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="V81" s="3">
         <v>2028</v>
@@ -4447,7 +4559,7 @@
         <v>999</v>
       </c>
       <c r="X81" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="82" spans="1:24">
@@ -4458,10 +4570,10 @@
         <v>71</v>
       </c>
       <c r="D82" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E82" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F82">
         <v>3000</v>
@@ -4470,7 +4582,7 @@
         <v>27</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I82">
         <v>100</v>
@@ -4479,10 +4591,10 @@
         <v>146</v>
       </c>
       <c r="N82" t="s">
+        <v>211</v>
+      </c>
+      <c r="O82" t="s">
         <v>212</v>
-      </c>
-      <c r="O82" t="s">
-        <v>213</v>
       </c>
       <c r="P82" s="1" t="s">
         <v>188</v>
@@ -4491,7 +4603,7 @@
         <v>9999999999</v>
       </c>
       <c r="R82" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="S82" t="s">
         <v>170</v>
@@ -4500,7 +4612,7 @@
         <v>19</v>
       </c>
       <c r="U82" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="V82" s="3">
         <v>2028</v>
@@ -4509,7 +4621,7 @@
         <v>999</v>
       </c>
       <c r="X82" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="91" spans="1:24" ht="15.6">
@@ -4520,7 +4632,7 @@
         <v>131</v>
       </c>
       <c r="D91" s="18" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="92" spans="1:24" ht="15.6">
@@ -4531,7 +4643,7 @@
         <v>161</v>
       </c>
       <c r="D92" s="18" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="93" spans="1:24" ht="15.6">
@@ -4539,10 +4651,10 @@
         <v>102</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D93" s="18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="94" spans="1:24" ht="15.6">
@@ -4550,10 +4662,10 @@
         <v>102</v>
       </c>
       <c r="C94" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D94" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="95" spans="1:24" ht="15.6">
@@ -4561,10 +4673,10 @@
         <v>102</v>
       </c>
       <c r="C95" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D95" s="18" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="97" spans="2:5" ht="15.6">
@@ -4575,7 +4687,7 @@
         <v>131</v>
       </c>
       <c r="D97" s="18" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="98" spans="2:5" ht="15.6">
@@ -4586,7 +4698,7 @@
         <v>161</v>
       </c>
       <c r="D98" s="18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="99" spans="2:5" ht="15.6">
@@ -4594,10 +4706,10 @@
         <v>109</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D99" s="18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="100" spans="2:5" ht="15.6">
@@ -4605,10 +4717,10 @@
         <v>109</v>
       </c>
       <c r="C100" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D100" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="101" spans="2:5" ht="15.6">
@@ -4616,10 +4728,10 @@
         <v>109</v>
       </c>
       <c r="C101" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D101" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="103" spans="2:5" ht="15.6">
@@ -4630,7 +4742,7 @@
         <v>131</v>
       </c>
       <c r="D103" s="18" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="104" spans="2:5" ht="15.6">
@@ -4641,7 +4753,7 @@
         <v>161</v>
       </c>
       <c r="D104" s="18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="105" spans="2:5" ht="15.6">
@@ -4649,10 +4761,10 @@
         <v>95</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D105" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="106" spans="2:5" ht="15.6">
@@ -4660,10 +4772,10 @@
         <v>95</v>
       </c>
       <c r="C106" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D106" s="18" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="107" spans="2:5" ht="15.6">
@@ -4671,15 +4783,15 @@
         <v>95</v>
       </c>
       <c r="C107" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D107" s="18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="109" spans="2:5">
       <c r="B109" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="111" spans="2:5">
@@ -4690,10 +4802,10 @@
         <v>131</v>
       </c>
       <c r="D111" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E111" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="112" spans="2:5">
@@ -4704,10 +4816,10 @@
         <v>161</v>
       </c>
       <c r="D112" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E112" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="113" spans="2:5">
@@ -4715,13 +4827,13 @@
         <v>71</v>
       </c>
       <c r="C113" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D113" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E113" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="114" spans="2:5">
@@ -4729,13 +4841,13 @@
         <v>71</v>
       </c>
       <c r="C114" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D114" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E114" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="115" spans="2:5">
@@ -4743,13 +4855,13 @@
         <v>71</v>
       </c>
       <c r="C115" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D115" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E115" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="117" spans="2:5" ht="15.6">
@@ -4760,10 +4872,10 @@
         <v>131</v>
       </c>
       <c r="D117" s="18" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E117" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="118" spans="2:5" ht="15.6">
@@ -4774,10 +4886,10 @@
         <v>161</v>
       </c>
       <c r="D118" s="18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E118" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="119" spans="2:5" ht="15.6">
@@ -4785,13 +4897,13 @@
         <v>102</v>
       </c>
       <c r="C119" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D119" s="18" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E119" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="120" spans="2:5" ht="15.6">
@@ -4799,13 +4911,13 @@
         <v>102</v>
       </c>
       <c r="C120" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D120" s="18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E120" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="121" spans="2:5" ht="15.6">
@@ -4813,13 +4925,13 @@
         <v>102</v>
       </c>
       <c r="C121" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D121" s="18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E121" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="123" spans="2:5" ht="15.6">
@@ -4830,10 +4942,10 @@
         <v>131</v>
       </c>
       <c r="D123" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E123" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="124" spans="2:5" ht="15.6">
@@ -4844,10 +4956,10 @@
         <v>161</v>
       </c>
       <c r="D124" s="18" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E124" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="125" spans="2:5" ht="15.6">
@@ -4855,13 +4967,13 @@
         <v>109</v>
       </c>
       <c r="C125" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D125" s="18" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E125" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="126" spans="2:5" ht="15.6">
@@ -4869,13 +4981,13 @@
         <v>109</v>
       </c>
       <c r="C126" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D126" s="18" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E126" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="127" spans="2:5" ht="15.6">
@@ -4883,13 +4995,13 @@
         <v>109</v>
       </c>
       <c r="C127" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D127" s="18" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E127" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="129" spans="1:46" ht="15.6">
@@ -4900,10 +5012,10 @@
         <v>131</v>
       </c>
       <c r="D129" s="18" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E129" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="130" spans="1:46" ht="15.6">
@@ -4914,10 +5026,10 @@
         <v>161</v>
       </c>
       <c r="D130" s="18" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E130" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="131" spans="1:46" ht="15.6">
@@ -4925,13 +5037,13 @@
         <v>95</v>
       </c>
       <c r="C131" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D131" s="18" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E131" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="132" spans="1:46" ht="15.6">
@@ -4939,13 +5051,13 @@
         <v>95</v>
       </c>
       <c r="C132" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D132" s="18" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E132" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="133" spans="1:46" ht="15.6">
@@ -4953,13 +5065,13 @@
         <v>95</v>
       </c>
       <c r="C133" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D133" s="18" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E133" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="138" spans="1:46" ht="16.8">
@@ -4973,7 +5085,7 @@
         <v>131</v>
       </c>
       <c r="F138" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G138">
         <v>24001</v>
@@ -4982,7 +5094,7 @@
         <v>27</v>
       </c>
       <c r="I138" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K138" t="s">
         <v>173</v>
@@ -5032,138 +5144,725 @@
         <v>0</v>
       </c>
       <c r="B140" s="20" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C140" s="20" t="s">
         <v>38</v>
       </c>
       <c r="D140" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="E140" s="20" t="s">
+        <v>312</v>
+      </c>
+      <c r="F140" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="G140" s="20" t="s">
         <v>314</v>
       </c>
-      <c r="E140" s="20" t="s">
+      <c r="H140" s="20" t="s">
         <v>315</v>
       </c>
-      <c r="F140" s="20" t="s">
+      <c r="I140" s="20" t="s">
         <v>316</v>
       </c>
-      <c r="G140" s="20" t="s">
+      <c r="J140" s="20" t="s">
         <v>317</v>
       </c>
-      <c r="H140" s="20" t="s">
+      <c r="K140" s="20" t="s">
         <v>318</v>
       </c>
-      <c r="I140" s="20" t="s">
+      <c r="L140" s="20" t="s">
         <v>319</v>
-      </c>
-      <c r="J140" s="20" t="s">
-        <v>320</v>
-      </c>
-      <c r="K140" s="20" t="s">
-        <v>321</v>
-      </c>
-      <c r="L140" s="20" t="s">
-        <v>322</v>
       </c>
       <c r="M140" s="20" t="s">
         <v>8</v>
       </c>
       <c r="N140" s="20" t="s">
+        <v>320</v>
+      </c>
+      <c r="O140" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="P140" s="20" t="s">
+        <v>322</v>
+      </c>
+      <c r="Q140" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="O140" s="20" t="s">
+      <c r="R140" s="20" t="s">
         <v>324</v>
       </c>
-      <c r="P140" s="20" t="s">
+      <c r="S140" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="Q140" s="20" t="s">
+      <c r="T140" s="20" t="s">
         <v>326</v>
       </c>
-      <c r="R140" s="20" t="s">
+      <c r="U140" s="20" t="s">
         <v>327</v>
       </c>
-      <c r="S140" s="20" t="s">
+      <c r="V140" s="20" t="s">
         <v>328</v>
       </c>
-      <c r="T140" s="20" t="s">
+      <c r="W140" s="20" t="s">
         <v>329</v>
       </c>
-      <c r="U140" s="20" t="s">
+      <c r="X140" s="20" t="s">
         <v>330</v>
       </c>
-      <c r="V140" s="20" t="s">
+      <c r="Y140" s="20" t="s">
         <v>331</v>
       </c>
-      <c r="W140" s="20" t="s">
+      <c r="Z140" s="20" t="s">
         <v>332</v>
       </c>
-      <c r="X140" s="20" t="s">
+      <c r="AA140" s="20" t="s">
         <v>333</v>
       </c>
-      <c r="Y140" s="20" t="s">
+      <c r="AB140" s="20" t="s">
         <v>334</v>
       </c>
-      <c r="Z140" s="20" t="s">
+      <c r="AC140" s="20" t="s">
         <v>335</v>
       </c>
-      <c r="AA140" s="20" t="s">
+      <c r="AD140" s="20" t="s">
         <v>336</v>
       </c>
-      <c r="AB140" s="20" t="s">
+      <c r="AE140" s="20" t="s">
         <v>337</v>
       </c>
-      <c r="AC140" s="20" t="s">
+      <c r="AF140" s="20" t="s">
         <v>338</v>
       </c>
-      <c r="AD140" s="20" t="s">
+      <c r="AG140" s="20" t="s">
         <v>339</v>
       </c>
-      <c r="AE140" s="20" t="s">
+      <c r="AH140" s="20" t="s">
         <v>340</v>
       </c>
-      <c r="AF140" s="20" t="s">
+      <c r="AI140" s="20" t="s">
         <v>341</v>
       </c>
-      <c r="AG140" s="20" t="s">
+      <c r="AJ140" s="21" t="s">
         <v>342</v>
       </c>
-      <c r="AH140" s="20" t="s">
+      <c r="AK140" s="21" t="s">
         <v>343</v>
       </c>
-      <c r="AI140" s="20" t="s">
+      <c r="AL140" s="21" t="s">
         <v>344</v>
       </c>
-      <c r="AJ140" s="21" t="s">
+      <c r="AM140" s="21" t="s">
         <v>345</v>
       </c>
-      <c r="AK140" s="21" t="s">
+      <c r="AN140" s="21" t="s">
         <v>346</v>
       </c>
-      <c r="AL140" s="21" t="s">
+      <c r="AO140" s="21" t="s">
         <v>347</v>
       </c>
-      <c r="AM140" s="21" t="s">
+      <c r="AP140" s="21" t="s">
         <v>348</v>
       </c>
-      <c r="AN140" s="21" t="s">
+      <c r="AQ140" s="21" t="s">
         <v>349</v>
       </c>
-      <c r="AO140" s="21" t="s">
+      <c r="AR140" s="21" t="s">
         <v>350</v>
       </c>
-      <c r="AP140" s="21" t="s">
+      <c r="AS140" s="21" t="s">
         <v>351</v>
       </c>
-      <c r="AQ140" s="21" t="s">
-        <v>352</v>
-      </c>
-      <c r="AR140" s="21" t="s">
+      <c r="AT140" s="3"/>
+    </row>
+    <row r="142" spans="1:46">
+      <c r="A142" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="144" spans="1:46" ht="16.8">
+      <c r="A144" s="3">
+        <v>1</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D144" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="E144" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F144" s="10"/>
+      <c r="G144" s="3">
+        <v>2000</v>
+      </c>
+      <c r="H144" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="I144" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="AS140" s="21" t="s">
-        <v>354</v>
-      </c>
-      <c r="AT140" s="3"/>
+      <c r="J144" s="3"/>
+      <c r="K144" s="3"/>
+      <c r="L144" s="3"/>
+      <c r="M144" s="3">
+        <v>10</v>
+      </c>
+      <c r="N144" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="O144" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="P144" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q144" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="R144" s="8">
+        <v>1234567890</v>
+      </c>
+      <c r="S144" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="T144" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="U144" s="22">
+        <v>4111111111111110</v>
+      </c>
+      <c r="V144" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="W144" s="3">
+        <v>2028</v>
+      </c>
+      <c r="X144" s="3">
+        <v>121</v>
+      </c>
+      <c r="Y144" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z144" s="3"/>
+      <c r="AA144" s="3"/>
+      <c r="AB144" s="3"/>
+    </row>
+    <row r="145" spans="1:29" ht="16.8">
+      <c r="A145" s="3">
+        <v>2</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="E145" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="F145" s="3"/>
+      <c r="G145" s="3">
+        <v>10000</v>
+      </c>
+      <c r="H145" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="I145" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="J145" s="3"/>
+      <c r="K145" s="3"/>
+      <c r="L145" s="3"/>
+      <c r="M145" s="3"/>
+      <c r="N145" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="O145" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="P145" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q145" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="R145" s="8">
+        <v>1234567890</v>
+      </c>
+      <c r="S145" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="T145" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="U145" s="22">
+        <v>4111111111111110</v>
+      </c>
+      <c r="V145" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="W145" s="3">
+        <v>2028</v>
+      </c>
+      <c r="X145" s="3">
+        <v>121</v>
+      </c>
+      <c r="Y145" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="Z145" s="3"/>
+      <c r="AA145" s="3"/>
+      <c r="AB145" s="3"/>
+    </row>
+    <row r="146" spans="1:29" ht="16.8">
+      <c r="A146" s="3">
+        <v>3</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D146" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="E146" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F146" s="10"/>
+      <c r="G146" s="3">
+        <v>2000</v>
+      </c>
+      <c r="H146" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="I146" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="J146" s="3"/>
+      <c r="K146" s="3"/>
+      <c r="L146" s="3"/>
+      <c r="M146" s="3">
+        <v>10</v>
+      </c>
+      <c r="N146" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="O146" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="P146" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q146" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="R146" s="8">
+        <v>1234567890</v>
+      </c>
+      <c r="S146" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="T146" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="U146" s="22">
+        <v>4111111111111110</v>
+      </c>
+      <c r="V146" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="W146" s="3">
+        <v>2028</v>
+      </c>
+      <c r="X146" s="3">
+        <v>121</v>
+      </c>
+      <c r="Y146" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z146" s="3"/>
+      <c r="AA146" s="3"/>
+      <c r="AB146" s="3"/>
+    </row>
+    <row r="147" spans="1:29" ht="16.8">
+      <c r="A147" s="3">
+        <v>4</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D147" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="E147" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="F147" s="3"/>
+      <c r="G147" s="3">
+        <v>10000</v>
+      </c>
+      <c r="H147" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="I147" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="J147" s="3"/>
+      <c r="K147" s="3"/>
+      <c r="L147" s="3"/>
+      <c r="M147" s="3"/>
+      <c r="N147" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="O147" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="P147" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q147" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="R147" s="8">
+        <v>1234567890</v>
+      </c>
+      <c r="S147" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="T147" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="U147" s="22">
+        <v>4111111111111110</v>
+      </c>
+      <c r="V147" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="W147" s="3">
+        <v>2028</v>
+      </c>
+      <c r="X147" s="3">
+        <v>121</v>
+      </c>
+      <c r="Y147" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="Z147" s="3"/>
+      <c r="AA147" s="3"/>
+      <c r="AB147" s="3"/>
+    </row>
+    <row r="149" spans="1:29" ht="18.600000000000001">
+      <c r="A149" s="3">
+        <v>1</v>
+      </c>
+      <c r="B149" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C149" s="3"/>
+      <c r="D149" s="3"/>
+      <c r="E149" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F149" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="G149" s="3">
+        <v>5000</v>
+      </c>
+      <c r="H149" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I149" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="J149" s="3"/>
+      <c r="K149" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L149" s="3"/>
+      <c r="M149" s="3">
+        <v>10</v>
+      </c>
+      <c r="N149" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="O149" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="P149" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q149" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="R149" s="8">
+        <v>9876543210</v>
+      </c>
+      <c r="S149" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="T149" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="U149" s="22">
+        <v>4111111111111110</v>
+      </c>
+      <c r="V149" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="W149" s="3">
+        <v>2026</v>
+      </c>
+      <c r="X149" s="3">
+        <v>121</v>
+      </c>
+      <c r="Y149" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="Z149" s="3"/>
+      <c r="AA149" s="16"/>
+      <c r="AB149" s="3"/>
+    </row>
+    <row r="150" spans="1:29" ht="18.600000000000001">
+      <c r="A150" s="3">
+        <v>2</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C150" s="3"/>
+      <c r="D150" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="E150" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F150" s="3"/>
+      <c r="G150" s="3">
+        <v>36001</v>
+      </c>
+      <c r="H150" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="I150" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="J150" s="3"/>
+      <c r="K150" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="L150" s="3"/>
+      <c r="M150" s="3"/>
+      <c r="N150" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="O150" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="P150" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q150" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="R150" s="8">
+        <v>9876543210</v>
+      </c>
+      <c r="S150" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="T150" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="U150" s="22">
+        <v>4111111111111110</v>
+      </c>
+      <c r="V150" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="W150" s="3">
+        <v>2026</v>
+      </c>
+      <c r="X150" s="3">
+        <v>121</v>
+      </c>
+      <c r="Y150" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="Z150" s="3"/>
+      <c r="AA150" s="16"/>
+      <c r="AB150" s="3"/>
+    </row>
+    <row r="152" spans="1:29" ht="18">
+      <c r="A152" s="3">
+        <v>1</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C152" s="24" t="s">
+        <v>376</v>
+      </c>
+      <c r="D152" s="23" t="s">
+        <v>377</v>
+      </c>
+      <c r="E152" s="3"/>
+      <c r="F152" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="G152" s="3">
+        <v>5000</v>
+      </c>
+      <c r="H152" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I152" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J152" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K152" s="25">
+        <v>0</v>
+      </c>
+      <c r="L152" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M152" s="3"/>
+      <c r="N152" s="3"/>
+      <c r="O152" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="P152" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q152" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="R152" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="S152" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="T152" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="U152" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="V152" s="22">
+        <v>4111111111111110</v>
+      </c>
+      <c r="W152" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="X152" s="3">
+        <v>2026</v>
+      </c>
+      <c r="Y152" s="3">
+        <v>121</v>
+      </c>
+      <c r="Z152" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="AA152" s="3"/>
+      <c r="AB152" s="14"/>
+      <c r="AC152" s="3"/>
+    </row>
+    <row r="153" spans="1:29" ht="18">
+      <c r="A153" s="3">
+        <v>2</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C153" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="D153" s="23" t="s">
+        <v>382</v>
+      </c>
+      <c r="E153" s="3"/>
+      <c r="F153" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="G153" s="3">
+        <v>35000</v>
+      </c>
+      <c r="H153" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="I153" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J153" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="K153" s="25">
+        <v>100</v>
+      </c>
+      <c r="L153" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="M153" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N153" s="3"/>
+      <c r="O153" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="P153" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q153" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="R153" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="S153" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="T153" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="U153" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="V153" s="22">
+        <v>4111111111111110</v>
+      </c>
+      <c r="W153" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="X153" s="3">
+        <v>2026</v>
+      </c>
+      <c r="Y153" s="3">
+        <v>121</v>
+      </c>
+      <c r="Z153" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA153" s="3"/>
+      <c r="AB153" s="14"/>
+      <c r="AC153" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5183,9 +5882,15 @@
     <hyperlink ref="P81" r:id="rId14" xr:uid="{9D7FCFEB-CE02-41CA-8A7A-C6F8BC91D5CC}"/>
     <hyperlink ref="P82" r:id="rId15" xr:uid="{97F15A86-B82F-4F68-8FE5-BC30CA476EAA}"/>
     <hyperlink ref="Q138" r:id="rId16" xr:uid="{3D93A652-F4D4-405F-A0A6-7016A2306BC1}"/>
+    <hyperlink ref="Q144" r:id="rId17" display="mailto:ganeshsase2020+4515@gmail.com" xr:uid="{CFBDE79C-0688-43F7-A500-8ADBB72B2F7F}"/>
+    <hyperlink ref="Q145" r:id="rId18" display="mailto:ganeshsase2020+4516@gmail.com" xr:uid="{8B485BFC-BC18-4836-98F7-4B2057DAFD5C}"/>
+    <hyperlink ref="Q146" r:id="rId19" display="mailto:ganeshsase2020+4517@gmail.com" xr:uid="{E1CCE7E2-9688-4E45-A43C-23A572F715D1}"/>
+    <hyperlink ref="Q147" r:id="rId20" display="mailto:ganeshsase2020+4518@gmail.com" xr:uid="{292AB5C4-ED46-4577-803F-A6F925B80A1D}"/>
+    <hyperlink ref="Q149" r:id="rId21" display="mailto:ganeshsase2020+4511@gmail.com" xr:uid="{8F59FAE4-96FE-4E10-9961-9361F3BDCC96}"/>
+    <hyperlink ref="Q150" r:id="rId22" display="mailto:ganeshsase2020+4512@gmail.com" xr:uid="{9FC18370-7D6B-45A8-A5A4-8A822455D19D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
 
@@ -5194,7 +5899,7 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5294,10 +5999,10 @@
         <v>2000</v>
       </c>
       <c r="H2" s="19" t="s">
+        <v>307</v>
+      </c>
+      <c r="I2" s="19" t="s">
         <v>308</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>309</v>
       </c>
       <c r="M2">
         <v>10</v>
@@ -5306,10 +6011,10 @@
         <v>128</v>
       </c>
       <c r="O2" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>212</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>213</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>188</v>
@@ -5327,7 +6032,7 @@
         <v>19</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="W2" s="3">
         <v>2028</v>
@@ -5351,15 +6056,255 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E2F5DD2-7F70-498E-8132-BA3482C4D469}">
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:AB3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:28">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" t="s">
+        <v>138</v>
+      </c>
+      <c r="N1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S1" t="s">
+        <v>58</v>
+      </c>
+      <c r="T1" t="s">
+        <v>75</v>
+      </c>
+      <c r="U1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W1" t="s">
+        <v>12</v>
+      </c>
+      <c r="X1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="16.8">
+      <c r="A2" s="3">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3">
+        <v>10000</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="R2" s="8">
+        <v>1234567890</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="U2" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="W2" s="3">
+        <v>2028</v>
+      </c>
+      <c r="X2" s="3">
+        <v>121</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:28" ht="16.8">
+      <c r="A3" s="3">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3">
+        <v>10000</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="R3" s="8">
+        <v>1234567890</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="U3" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="W3" s="3">
+        <v>2028</v>
+      </c>
+      <c r="X3" s="3">
+        <v>121</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="Q2" r:id="rId1" display="mailto:ganeshsase2020+4516@gmail.com" xr:uid="{80CF806E-F005-4A9F-83E7-6C737ABBE0F8}"/>
+    <hyperlink ref="Q3" r:id="rId2" display="mailto:ganeshsase2020+4518@gmail.com" xr:uid="{F666636E-5017-4D76-8106-8AB16AE577FB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB7AC2E-A463-44B1-9F21-06F4E148C279}">
+  <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:27">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -5391,290 +6336,129 @@
         <v>63</v>
       </c>
       <c r="K1" t="s">
+        <v>178</v>
+      </c>
+      <c r="L1" t="s">
         <v>62</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>61</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>138</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>59</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>4</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>55</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>56</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>57</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>58</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>75</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>10</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>11</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>12</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>13</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="16.8">
+    <row r="2" spans="1:27" ht="16.8">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="D2" t="s">
-        <v>357</v>
+      <c r="B2" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="27" t="s">
+        <v>387</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="F2" s="10"/>
+        <v>131</v>
+      </c>
+      <c r="F2" s="3"/>
       <c r="G2" s="3">
-        <v>2000</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>308</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>309</v>
-      </c>
-      <c r="M2">
-        <v>10</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>128</v>
-      </c>
+        <v>13000</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="J2" s="23">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="M2" s="3"/>
       <c r="O2" s="3" t="s">
-        <v>212</v>
+        <v>122</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="R2" s="8">
-        <v>4044063049</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="S2" s="8">
+        <v>1234567890</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="U2" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="V2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="V2" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="W2" s="3">
-        <v>2028</v>
+      <c r="W2" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="X2" s="3">
+        <v>2029</v>
+      </c>
+      <c r="Y2" s="3">
         <v>121</v>
       </c>
-      <c r="Y2" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="Z2" s="3"/>
+      <c r="Z2" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA2" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Q2" r:id="rId1" xr:uid="{B621DC52-1F81-4870-B211-0D0D750EE929}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB7AC2E-A463-44B1-9F21-06F4E148C279}">
-  <dimension ref="A1:Z2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1" spans="1:26">
-      <c r="A1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H1" t="s">
-        <v>65</v>
-      </c>
-      <c r="I1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" t="s">
-        <v>63</v>
-      </c>
-      <c r="K1" t="s">
-        <v>178</v>
-      </c>
-      <c r="L1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M1" t="s">
-        <v>61</v>
-      </c>
-      <c r="N1" t="s">
-        <v>138</v>
-      </c>
-      <c r="O1" t="s">
-        <v>59</v>
-      </c>
-      <c r="P1" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>55</v>
-      </c>
-      <c r="R1" t="s">
-        <v>56</v>
-      </c>
-      <c r="S1" t="s">
-        <v>57</v>
-      </c>
-      <c r="T1" t="s">
-        <v>58</v>
-      </c>
-      <c r="U1" t="s">
-        <v>75</v>
-      </c>
-      <c r="V1" t="s">
-        <v>10</v>
-      </c>
-      <c r="W1" t="s">
-        <v>11</v>
-      </c>
-      <c r="X1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" ht="16.8">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="E2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G2">
-        <v>36001</v>
-      </c>
-      <c r="H2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="J2" s="7">
-        <v>100</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3">
-        <v>10</v>
-      </c>
-      <c r="O2" t="s">
-        <v>52</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="S2" s="8">
-        <v>1111111111</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="X2" s="3">
-        <v>2029</v>
-      </c>
-      <c r="Y2" s="3">
-        <v>121</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="R2" r:id="rId1" xr:uid="{2727FAFF-CC2B-407A-82DE-9C7002C4EE4A}"/>
+    <hyperlink ref="R2" r:id="rId1" display="mailto:ganeshsase2020+4513@gmail.com" xr:uid="{C3786877-4EDD-4228-9A23-DEF4D562A206}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -5683,15 +6467,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C81B7B-8FF9-4DAF-A14D-5ECF2C456AD0}">
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:29">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -5771,40 +6555,43 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:29" ht="30">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="F2" t="s">
-        <v>311</v>
-      </c>
-      <c r="G2">
-        <v>24001</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="C2" s="24" t="s">
+        <v>376</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>377</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="G2" s="3">
+        <v>5000</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="I2" t="s">
-        <v>127</v>
+      <c r="I2" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="K2" s="11">
-        <v>250</v>
-      </c>
-      <c r="L2" t="s">
-        <v>173</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="K2" s="25">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
       <c r="O2" s="3" t="s">
         <v>122</v>
       </c>
@@ -5814,54 +6601,56 @@
       <c r="Q2" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="R2" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="S2" s="8">
-        <v>1111111111</v>
+      <c r="R2" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>380</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>137</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="V2" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="V2" s="28" t="s">
         <v>19</v>
       </c>
       <c r="W2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="X2">
+      <c r="X2" s="3">
         <v>2026</v>
       </c>
       <c r="Y2" s="3">
         <v>121</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Z2" s="27" t="s">
         <v>137</v>
       </c>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="3"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="R2" r:id="rId1" display="dipakgaondhare11+7111@gmail.com" xr:uid="{D405792F-D753-4487-9F56-9A4A7C963B12}"/>
-    <hyperlink ref="R2" r:id="rId2" display="ganeshsase2020+2705@gmail.com" xr:uid="{E5AD1BEF-FC29-40A2-9C1B-46C02D1BD8B4}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDE93E67-3923-4C95-BAC6-6654B250474C}">
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="21" max="21" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:28">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -5938,32 +6727,36 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="16.8">
+    <row r="2" spans="1:28" ht="18.600000000000001">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="F2" t="s">
-        <v>261</v>
-      </c>
-      <c r="G2">
-        <v>24001</v>
+      <c r="F2" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="G2" s="3">
+        <v>5000</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="K2" t="s">
-        <v>173</v>
-      </c>
-      <c r="M2">
+      <c r="I2" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3">
         <v>10</v>
       </c>
       <c r="N2" s="3" t="s">
@@ -5976,16 +6769,16 @@
         <v>184</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>188</v>
+        <v>368</v>
       </c>
       <c r="R2" s="8">
-        <v>1111111112</v>
+        <v>9999999999</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>137</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="U2" s="4" t="s">
         <v>19</v>
@@ -5994,21 +6787,93 @@
         <v>17</v>
       </c>
       <c r="W2" s="3">
-        <v>2029</v>
+        <v>2026</v>
       </c>
       <c r="X2" s="3">
         <v>121</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>137</v>
-      </c>
+        <v>369</v>
+      </c>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="16"/>
+      <c r="AB2" s="3"/>
+    </row>
+    <row r="3" spans="1:28" ht="18.600000000000001">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3">
+        <v>36001</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="R3" s="8">
+        <v>9999999999</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="W3" s="3">
+        <v>2026</v>
+      </c>
+      <c r="X3" s="3">
+        <v>121</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="16"/>
+      <c r="AB3" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Q2" r:id="rId1" xr:uid="{79D25B07-FC44-4D2B-BAD7-1FFA98017A7D}"/>
+    <hyperlink ref="Q2" r:id="rId1" display="mailto:ganeshsase2020+4511@gmail.com" xr:uid="{69EAE568-3425-4095-8752-A5B57AA04B39}"/>
+    <hyperlink ref="Q3" r:id="rId2" display="mailto:ganeshsase2020+4512@gmail.com" xr:uid="{8DD5B121-B299-4EA8-AEF0-FA3291007EAE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -6016,7 +6881,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC174C8-7337-48DF-B748-6BE368B466D0}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>

</xml_diff>